<commit_message>
New Excel file structure
Updaste Posts.xlsx
</commit_message>
<xml_diff>
--- a/admin/data/Posts.xlsx
+++ b/admin/data/Posts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Craft\Documents\java\theatertage\admin\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schar\OneDrive\Dokumente\GitHub\theatertage\admin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56D7E7B-F858-4700-9220-02F167022850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9200F2B-F820-42E9-90F1-7946B4BFC906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34875" yWindow="3180" windowWidth="28800" windowHeight="15435" xr2:uid="{256E3240-CDF5-4972-A2EE-7B5DB3DA5C5C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="35314" windowHeight="18720" xr2:uid="{256E3240-CDF5-4972-A2EE-7B5DB3DA5C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Newsletter" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="38">
   <si>
     <t>img1</t>
   </si>
@@ -74,18 +74,6 @@
     <t>sum</t>
   </si>
   <si>
-    <t>t1</t>
-  </si>
-  <si>
-    <t>t2</t>
-  </si>
-  <si>
-    <t>t3</t>
-  </si>
-  <si>
-    <t>t4</t>
-  </si>
-  <si>
     <t>i1</t>
   </si>
   <si>
@@ -123,6 +111,45 @@
   </si>
   <si>
     <t>summary 1</t>
+  </si>
+  <si>
+    <t>head1</t>
+  </si>
+  <si>
+    <t>head2</t>
+  </si>
+  <si>
+    <t>head3</t>
+  </si>
+  <si>
+    <t>head4</t>
+  </si>
+  <si>
+    <t>Mini-Headline1</t>
+  </si>
+  <si>
+    <t>Mini-Headline2</t>
+  </si>
+  <si>
+    <t>Mini-Headline3</t>
+  </si>
+  <si>
+    <t>Mini-Headline4</t>
+  </si>
+  <si>
+    <t>author1</t>
+  </si>
+  <si>
+    <t>author2</t>
+  </si>
+  <si>
+    <t>author3</t>
+  </si>
+  <si>
+    <t>author4</t>
+  </si>
+  <si>
+    <t>Anonym</t>
   </si>
 </sst>
 </file>
@@ -169,7 +196,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -501,18 +528,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99764E3C-1248-44C0-80ED-9F1AB2E0971D}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -532,22 +559,46 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>45314</v>
       </c>
@@ -555,174 +606,294 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>45315</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>45316</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>45317</v>
       </c>
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>45318</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="H7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further progress with Newsletter
</commit_message>
<xml_diff>
--- a/admin/data/Posts.xlsx
+++ b/admin/data/Posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schar\Documents\GitHub\theatertage\admin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7799149-C4FF-41FF-A726-E659A30D93DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1324166C-EDC9-4B87-BB92-732927C7F575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{256E3240-CDF5-4972-A2EE-7B5DB3DA5C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="52">
   <si>
     <t>img1</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Die Nutzung der App ist aus der Sicht von Experten aus weiteren Gründen problematisch. Nicht nur, weil TikTok sehr viele Daten über seine Nutzer sammelt, sondern auch, weil eine übermäßige Nutzung der Plattform zu massivem Suchtverhalten führen kann, welches den gesamten Alltag von Jugendlichen beherrschen kann. \n So wird beispielsweise die Kapazität deines Arbeitsgedächtnisses durch TikTok-Nutzern reduziert. Das bedeutet, dass man dadurch aktiv „verdummt“. Deshalb hat man oft keine Lust mehr, über einen längeren Zeitraum etwas anderes zu tun oder sich zu konzentrieren. Man kann/will z.B. Konversationen nicht mehr aufmerksam zuhören. Das alles funktioniert, weil die Nutzer durch TikTok kurzfristige positive Rückmeldungen bekommen, wie bei einer Art Belohnung. Dabei sind es im wirklichen Leben die langfristigen Belohnungen, die einen glücklich machen, z.B. mit der Familie etwas zu unternehmen. \n Nicht nur die Art, wie TikTok seine User an sich bindet, kann schädlich sein, sondern auch, welcher Content auf den Nutzer zugeschnitten wird. Ein großer Nachteil ist zudem, dass bei süchtigen TikTok-Nutzern Depressionen, Angst und Stress auftreten können. Wenn man z.B. schon solche Tendenzen zeigt, werden Stimmungen wie Traurigkeit durch thematisch zugeschnittene Videos auf TikTok zusätzlich unterstützt. Damit ist TikTok nicht nur für die mentale Gesundheit des Einzelnen, sondern auch für uns als Gesellschaft eine große Gefahr. \n Dass TikTok weiterreichende Auswirkungen auf unsere Jugend, unsere Psyche und unsere Gesellschaft hat, sollte dir spätestens jetzt bewusst sein. Was hältst du von TikTok? Schreib‘ uns deine Meinung: schuelerzeitung@gmg.amberg.de</t>
+  </si>
+  <si>
+    <t>author5</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99764E3C-1248-44C0-80ED-9F1AB2E0971D}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +581,7 @@
     <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -636,8 +639,11 @@
       <c r="S1" t="s">
         <v>10</v>
       </c>
+      <c r="T1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45314</v>
       </c>
@@ -695,8 +701,11 @@
       <c r="S2" t="s">
         <v>50</v>
       </c>
+      <c r="T2" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45315</v>
       </c>
@@ -754,8 +763,11 @@
       <c r="S3" t="s">
         <v>19</v>
       </c>
+      <c r="T3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45316</v>
       </c>
@@ -813,8 +825,11 @@
       <c r="S4" t="s">
         <v>20</v>
       </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45317</v>
       </c>
@@ -872,8 +887,11 @@
       <c r="S5" t="s">
         <v>21</v>
       </c>
+      <c r="T5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45318</v>
       </c>
@@ -931,8 +949,11 @@
       <c r="S6" t="s">
         <v>22</v>
       </c>
+      <c r="T6" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
idea for paragraph structure in blogpost summary
</commit_message>
<xml_diff>
--- a/admin/data/Posts.xlsx
+++ b/admin/data/Posts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schar\Documents\GitHub\theatertage\admin\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schar\OneDrive\Dokumente\GitHub\theatertage\admin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1324166C-EDC9-4B87-BB92-732927C7F575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554B04CB-97AC-405A-AA4C-14D87A228297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{256E3240-CDF5-4972-A2EE-7B5DB3DA5C5C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="35314" windowHeight="18720" xr2:uid="{256E3240-CDF5-4972-A2EE-7B5DB3DA5C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Newsletter" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="55">
   <si>
     <t>img1</t>
   </si>
@@ -188,10 +188,19 @@
     <t>Vor allem junge Mädchen möchten damit viele Follower generieren, weshalb sie sich manchmal sogar knapp bekleidet filmen oder provokante Tanzvideos veröffentlichen. Damit werden gerade Männer angesprochen, die den Mädchen dann oft folgen und sie kontaktieren. Die Mädchen fühlen sich geschmeichelt und unterschätzen die Gefahr dieser Kontakte. Und das tun sie alles nur, um Follower zu bekommen.</t>
   </si>
   <si>
-    <t>Die Nutzung der App ist aus der Sicht von Experten aus weiteren Gründen problematisch. Nicht nur, weil TikTok sehr viele Daten über seine Nutzer sammelt, sondern auch, weil eine übermäßige Nutzung der Plattform zu massivem Suchtverhalten führen kann, welches den gesamten Alltag von Jugendlichen beherrschen kann. \n So wird beispielsweise die Kapazität deines Arbeitsgedächtnisses durch TikTok-Nutzern reduziert. Das bedeutet, dass man dadurch aktiv „verdummt“. Deshalb hat man oft keine Lust mehr, über einen längeren Zeitraum etwas anderes zu tun oder sich zu konzentrieren. Man kann/will z.B. Konversationen nicht mehr aufmerksam zuhören. Das alles funktioniert, weil die Nutzer durch TikTok kurzfristige positive Rückmeldungen bekommen, wie bei einer Art Belohnung. Dabei sind es im wirklichen Leben die langfristigen Belohnungen, die einen glücklich machen, z.B. mit der Familie etwas zu unternehmen. \n Nicht nur die Art, wie TikTok seine User an sich bindet, kann schädlich sein, sondern auch, welcher Content auf den Nutzer zugeschnitten wird. Ein großer Nachteil ist zudem, dass bei süchtigen TikTok-Nutzern Depressionen, Angst und Stress auftreten können. Wenn man z.B. schon solche Tendenzen zeigt, werden Stimmungen wie Traurigkeit durch thematisch zugeschnittene Videos auf TikTok zusätzlich unterstützt. Damit ist TikTok nicht nur für die mentale Gesundheit des Einzelnen, sondern auch für uns als Gesellschaft eine große Gefahr. \n Dass TikTok weiterreichende Auswirkungen auf unsere Jugend, unsere Psyche und unsere Gesellschaft hat, sollte dir spätestens jetzt bewusst sein. Was hältst du von TikTok? Schreib‘ uns deine Meinung: schuelerzeitung@gmg.amberg.de</t>
-  </si>
-  <si>
     <t>author5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So wird beispielsweise die Kapazität deines Arbeitsgedächtnisses durch TikTok-Nutzern reduziert. Das bedeutet, dass man dadurch aktiv „verdummt“. Deshalb hat man oft keine Lust mehr, über einen längeren Zeitraum etwas anderes zu tun oder sich zu konzentrieren. Man kann/will z.B. Konversationen nicht mehr aufmerksam zuhören. Das alles funktioniert, weil die Nutzer durch TikTok kurzfristige positive Rückmeldungen bekommen, wie bei einer Art Belohnung. Dabei sind es im wirklichen Leben die langfristigen Belohnungen, die einen glücklich machen, z.B. mit der Familie etwas zu unternehmen. </t>
+  </si>
+  <si>
+    <t>Nicht nur die Art, wie TikTok seine User an sich bindet, kann schädlich sein, sondern auch, welcher Content auf den Nutzer zugeschnitten wird. Ein großer Nachteil ist zudem, dass bei süchtigen TikTok-Nutzern Depressionen, Angst und Stress auftreten können. Wenn man z.B. schon solche Tendenzen zeigt, werden Stimmungen wie Traurigkeit durch thematisch zugeschnittene Videos auf TikTok zusätzlich unterstützt. Damit ist TikTok nicht nur für die mentale Gesundheit des Einzelnen, sondern auch für uns als Gesellschaft eine große Gefahr.</t>
+  </si>
+  <si>
+    <t>Dass TikTok weiterreichende Auswirkungen auf unsere Jugend, unsere Psyche und unsere Gesellschaft hat, sollte dir spätestens jetzt bewusst sein. Was hältst du von TikTok? Schreib‘ uns deine Meinung: schuelerzeitung@gmg.amberg.de</t>
+  </si>
+  <si>
+    <t>Die Nutzung der App ist aus der Sicht von Experten aus weiteren Gründen problematisch. Nicht nur, weil TikTok sehr viele Daten über seine Nutzer sammelt, sondern auch, weil eine übermäßige Nutzung der Plattform zu massivem Suchtverhalten führen kann, welches den gesamten Alltag von Jugendlichen beherrschen kann.</t>
   </si>
 </sst>
 </file>
@@ -238,7 +247,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -570,18 +579,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99764E3C-1248-44C0-80ED-9F1AB2E0971D}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -637,13 +646,13 @@
         <v>34</v>
       </c>
       <c r="S1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" t="s">
         <v>10</v>
       </c>
-      <c r="T1" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>45314</v>
       </c>
@@ -699,13 +708,22 @@
         <v>45</v>
       </c>
       <c r="S2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="T2" t="s">
-        <v>35</v>
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
+        <v>51</v>
+      </c>
+      <c r="V2" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>45315</v>
       </c>
@@ -761,13 +779,13 @@
         <v>35</v>
       </c>
       <c r="S3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" t="s">
         <v>19</v>
       </c>
-      <c r="T3" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>45316</v>
       </c>
@@ -823,13 +841,13 @@
         <v>35</v>
       </c>
       <c r="S4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" t="s">
         <v>20</v>
       </c>
-      <c r="T4" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>45317</v>
       </c>
@@ -885,13 +903,13 @@
         <v>35</v>
       </c>
       <c r="S5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" t="s">
         <v>21</v>
       </c>
-      <c r="T5" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>45318</v>
       </c>
@@ -947,13 +965,13 @@
         <v>35</v>
       </c>
       <c r="S6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" t="s">
         <v>22</v>
       </c>
-      <c r="T6" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
       <c r="H7" s="1"/>
     </row>
   </sheetData>

</xml_diff>